<commit_message>
Updated 운동기록.png and 운동기록.xlsx
</commit_message>
<xml_diff>
--- a/exercise/운동기록.xlsx
+++ b/exercise/운동기록.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Seung Jae Han\Dropbox\Trivia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9E1F884-1FEE-46C4-97E2-16960D09083D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E54A1777-F2E1-4E0F-B485-77787FDD2C41}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="15">
   <si>
     <t>DATETIME</t>
   </si>
@@ -432,11 +432,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I20"/>
+  <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F13" sqref="F13"/>
+      <selection pane="bottomLeft" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1029,6 +1029,35 @@
         <v>12</v>
       </c>
     </row>
+    <row r="21" spans="1:9">
+      <c r="A21" s="2">
+        <v>44006</v>
+      </c>
+      <c r="B21" s="3">
+        <v>100</v>
+      </c>
+      <c r="C21" s="3">
+        <v>106</v>
+      </c>
+      <c r="D21" s="3">
+        <v>0.9</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F21" s="3">
+        <v>0</v>
+      </c>
+      <c r="G21" s="3">
+        <v>82.1</v>
+      </c>
+      <c r="H21" s="3">
+        <v>28.7</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated 운동기록.png and 운동기록.xslx
</commit_message>
<xml_diff>
--- a/exercise/운동기록.xlsx
+++ b/exercise/운동기록.xlsx
@@ -8,19 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Seung Jae Han\Dropbox\Trivia\운동기록\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D99705B-6417-4CD7-B57C-8B1A218177FA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E138D392-C76E-4315-8B54-16780E767A13}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4800" yWindow="0" windowWidth="14400" windowHeight="7360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="운동기록" sheetId="1" r:id="rId1"/>
+    <sheet name="SEUNGJAE_HAN.&quot;운동기록&quot;" sheetId="1" r:id="rId1"/>
+    <sheet name="SQL" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="19">
   <si>
     <t>DATETIME</t>
   </si>
@@ -74,6 +75,9 @@
   </si>
   <si>
     <t>WORSENED</t>
+  </si>
+  <si>
+    <t>select DATETIME DATETIME, WAIST WAIST, HIP HIP, WHR WHR, WHR_IMPROVEMENT WHR_IMPROVEMENT, WHR_CHANGE WHR_CHANGE, WEIGHT WEIGHT, WHTR WHTR, WHTR_IMPROVEMENT WHTR_IMPROVEMENT, WHTR_CHANGE WHTR_CHANGE, BMI BMI, OBESITY OBESITY from (select * from "SEUNGJAE_HAN"."운동기록")</t>
   </si>
 </sst>
 </file>
@@ -441,7 +445,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L27"/>
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:L28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -1484,6 +1491,62 @@
         <v>16</v>
       </c>
     </row>
+    <row r="28" spans="1:12">
+      <c r="A28" s="2">
+        <v>44013</v>
+      </c>
+      <c r="B28" s="3">
+        <v>97.5</v>
+      </c>
+      <c r="C28" s="3">
+        <v>104.5</v>
+      </c>
+      <c r="D28" s="3">
+        <v>0.93</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F28" s="3">
+        <v>0</v>
+      </c>
+      <c r="G28" s="3">
+        <v>82.6</v>
+      </c>
+      <c r="H28" s="3">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="I28" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J28" s="3">
+        <v>0</v>
+      </c>
+      <c r="K28" s="3">
+        <v>28.9</v>
+      </c>
+      <c r="L28" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetData>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated 운동기록.sql, 운동기록.png, and 운동기록.xlsx
I adjusted my height from 169cm to 169.7cm
</commit_message>
<xml_diff>
--- a/exercise/운동기록.xlsx
+++ b/exercise/운동기록.xlsx
@@ -8,20 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Seung Jae Han\Dropbox\Trivia\운동기록\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E138D392-C76E-4315-8B54-16780E767A13}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8FC5E57-0341-47F6-AD96-3DEA0E9D67F2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4800" yWindow="0" windowWidth="14400" windowHeight="7360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="SEUNGJAE_HAN.&quot;운동기록&quot;" sheetId="1" r:id="rId1"/>
-    <sheet name="SQL" sheetId="2" r:id="rId2"/>
+    <sheet name="운동기록" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="18">
   <si>
     <t>DATETIME</t>
   </si>
@@ -75,9 +74,6 @@
   </si>
   <si>
     <t>WORSENED</t>
-  </si>
-  <si>
-    <t>select DATETIME DATETIME, WAIST WAIST, HIP HIP, WHR WHR, WHR_IMPROVEMENT WHR_IMPROVEMENT, WHR_CHANGE WHR_CHANGE, WEIGHT WEIGHT, WHTR WHTR, WHTR_IMPROVEMENT WHTR_IMPROVEMENT, WHTR_CHANGE WHTR_CHANGE, BMI BMI, OBESITY OBESITY from (select * from "SEUNGJAE_HAN"."운동기록")</t>
   </si>
 </sst>
 </file>
@@ -445,14 +441,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr>
-    <pageSetUpPr fitToPage="1"/>
-  </sheetPr>
-  <dimension ref="A1:L28"/>
+  <dimension ref="A1:L30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:XFD1048576"/>
+      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -529,7 +522,7 @@
         <v>12</v>
       </c>
       <c r="H2" s="3">
-        <v>0.62</v>
+        <v>0.61</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>12</v>
@@ -564,7 +557,7 @@
         <v>12</v>
       </c>
       <c r="H3" s="3">
-        <v>0.62</v>
+        <v>0.61</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>15</v>
@@ -608,10 +601,10 @@
         <v>14</v>
       </c>
       <c r="J4" s="3">
-        <v>0.03</v>
+        <v>0.02</v>
       </c>
       <c r="K4" s="3">
-        <v>28.9</v>
+        <v>28.7</v>
       </c>
       <c r="L4" s="1" t="s">
         <v>16</v>
@@ -640,16 +633,16 @@
         <v>83</v>
       </c>
       <c r="H5" s="3">
-        <v>0.59</v>
+        <v>0.57999999999999996</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J5" s="3">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="K5" s="3">
-        <v>29.1</v>
+        <v>28.8</v>
       </c>
       <c r="L5" s="1" t="s">
         <v>16</v>
@@ -681,13 +674,13 @@
         <v>0.59</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="J6" s="3">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="K6" s="3">
-        <v>28.7</v>
+        <v>28.5</v>
       </c>
       <c r="L6" s="1" t="s">
         <v>16</v>
@@ -716,16 +709,16 @@
         <v>82.5</v>
       </c>
       <c r="H7" s="3">
-        <v>0.6</v>
+        <v>0.59</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="J7" s="3">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="K7" s="3">
-        <v>28.9</v>
+        <v>28.6</v>
       </c>
       <c r="L7" s="1" t="s">
         <v>16</v>
@@ -760,10 +753,10 @@
         <v>14</v>
       </c>
       <c r="J8" s="3">
-        <v>0.02</v>
+        <v>0.01</v>
       </c>
       <c r="K8" s="3">
-        <v>28.7</v>
+        <v>28.4</v>
       </c>
       <c r="L8" s="1" t="s">
         <v>16</v>
@@ -792,16 +785,16 @@
         <v>82.2</v>
       </c>
       <c r="H9" s="3">
-        <v>0.59</v>
+        <v>0.57999999999999996</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="J9" s="3">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="K9" s="3">
-        <v>28.8</v>
+        <v>28.5</v>
       </c>
       <c r="L9" s="1" t="s">
         <v>16</v>
@@ -833,13 +826,13 @@
         <v>0.57999999999999996</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="J10" s="3">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="K10" s="3">
-        <v>28.9</v>
+        <v>28.6</v>
       </c>
       <c r="L10" s="1" t="s">
         <v>16</v>
@@ -877,7 +870,7 @@
         <v>0.01</v>
       </c>
       <c r="K11" s="3">
-        <v>28.8</v>
+        <v>28.6</v>
       </c>
       <c r="L11" s="1" t="s">
         <v>16</v>
@@ -915,7 +908,7 @@
         <v>0</v>
       </c>
       <c r="K12" s="3">
-        <v>28.9</v>
+        <v>28.6</v>
       </c>
       <c r="L12" s="1" t="s">
         <v>16</v>
@@ -953,7 +946,7 @@
         <v>0</v>
       </c>
       <c r="K13" s="3">
-        <v>29</v>
+        <v>28.7</v>
       </c>
       <c r="L13" s="1" t="s">
         <v>16</v>
@@ -991,7 +984,7 @@
         <v>0.01</v>
       </c>
       <c r="K14" s="3">
-        <v>29.2</v>
+        <v>29</v>
       </c>
       <c r="L14" s="1" t="s">
         <v>16</v>
@@ -1029,7 +1022,7 @@
         <v>0</v>
       </c>
       <c r="K15" s="3">
-        <v>29.2</v>
+        <v>28.9</v>
       </c>
       <c r="L15" s="1" t="s">
         <v>16</v>
@@ -1058,16 +1051,16 @@
         <v>82.1</v>
       </c>
       <c r="H16" s="3">
-        <v>0.59</v>
+        <v>0.57999999999999996</v>
       </c>
       <c r="I16" s="1" t="s">
         <v>14</v>
       </c>
       <c r="J16" s="3">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
       <c r="K16" s="3">
-        <v>28.7</v>
+        <v>28.5</v>
       </c>
       <c r="L16" s="1" t="s">
         <v>16</v>
@@ -1099,13 +1092,13 @@
         <v>0.57999999999999996</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="J17" s="3">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="K17" s="3">
-        <v>28.5</v>
+        <v>28.3</v>
       </c>
       <c r="L17" s="1" t="s">
         <v>16</v>
@@ -1143,7 +1136,7 @@
         <v>0.01</v>
       </c>
       <c r="K18" s="3">
-        <v>28.6</v>
+        <v>28.4</v>
       </c>
       <c r="L18" s="1" t="s">
         <v>16</v>
@@ -1181,7 +1174,7 @@
         <v>0</v>
       </c>
       <c r="K19" s="3">
-        <v>29.1</v>
+        <v>28.8</v>
       </c>
       <c r="L19" s="1" t="s">
         <v>16</v>
@@ -1219,7 +1212,7 @@
         <v>0</v>
       </c>
       <c r="K20" s="3">
-        <v>28.9</v>
+        <v>28.7</v>
       </c>
       <c r="L20" s="1" t="s">
         <v>16</v>
@@ -1257,7 +1250,7 @@
         <v>0</v>
       </c>
       <c r="K21" s="3">
-        <v>28.7</v>
+        <v>28.5</v>
       </c>
       <c r="L21" s="1" t="s">
         <v>16</v>
@@ -1286,16 +1279,16 @@
         <v>82.4</v>
       </c>
       <c r="H22" s="3">
-        <v>0.59</v>
+        <v>0.57999999999999996</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J22" s="3">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="K22" s="3">
-        <v>28.9</v>
+        <v>28.6</v>
       </c>
       <c r="L22" s="1" t="s">
         <v>16</v>
@@ -1327,13 +1320,13 @@
         <v>0.59</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="J23" s="3">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="K23" s="3">
-        <v>28.9</v>
+        <v>28.7</v>
       </c>
       <c r="L23" s="1" t="s">
         <v>16</v>
@@ -1371,7 +1364,7 @@
         <v>0.01</v>
       </c>
       <c r="K24" s="3">
-        <v>29.2</v>
+        <v>28.9</v>
       </c>
       <c r="L24" s="1" t="s">
         <v>16</v>
@@ -1409,7 +1402,7 @@
         <v>0</v>
       </c>
       <c r="K25" s="3">
-        <v>29.3</v>
+        <v>29.1</v>
       </c>
       <c r="L25" s="1" t="s">
         <v>16</v>
@@ -1438,16 +1431,16 @@
         <v>82.7</v>
       </c>
       <c r="H26" s="3">
-        <v>0.57999999999999996</v>
+        <v>0.56999999999999995</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J26" s="3">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="K26" s="3">
-        <v>29</v>
+        <v>28.7</v>
       </c>
       <c r="L26" s="1" t="s">
         <v>16</v>
@@ -1479,13 +1472,13 @@
         <v>0.57999999999999996</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="J27" s="3">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="K27" s="3">
-        <v>28.9</v>
+        <v>28.6</v>
       </c>
       <c r="L27" s="1" t="s">
         <v>16</v>
@@ -1514,37 +1507,95 @@
         <v>82.6</v>
       </c>
       <c r="H28" s="3">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="I28" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J28" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="K28" s="3">
+        <v>28.7</v>
+      </c>
+      <c r="L28" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12">
+      <c r="A29" s="2">
+        <v>44014</v>
+      </c>
+      <c r="B29" s="3">
+        <v>99.5</v>
+      </c>
+      <c r="C29" s="3">
+        <v>105.5</v>
+      </c>
+      <c r="D29" s="3">
+        <v>0.94</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F29" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="G29" s="3">
+        <v>82.4</v>
+      </c>
+      <c r="H29" s="3">
+        <v>0.59</v>
+      </c>
+      <c r="I29" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J29" s="3">
+        <v>0.02</v>
+      </c>
+      <c r="K29" s="3">
+        <v>28.6</v>
+      </c>
+      <c r="L29" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12">
+      <c r="A30" s="2">
+        <v>44015</v>
+      </c>
+      <c r="B30" s="3">
+        <v>98.5</v>
+      </c>
+      <c r="C30" s="3">
+        <v>104.5</v>
+      </c>
+      <c r="D30" s="3">
+        <v>0.94</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F30" s="3">
+        <v>0</v>
+      </c>
+      <c r="G30" s="3">
+        <v>81.5</v>
+      </c>
+      <c r="H30" s="3">
         <v>0.57999999999999996</v>
       </c>
-      <c r="I28" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="J28" s="3">
-        <v>0</v>
-      </c>
-      <c r="K28" s="3">
-        <v>28.9</v>
-      </c>
-      <c r="L28" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
-  <sheetData>
-    <row r="2" spans="1:1">
-      <c r="A2" t="s">
-        <v>18</v>
+      <c r="I30" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J30" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="K30" s="3">
+        <v>28.3</v>
+      </c>
+      <c r="L30" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated 운동기록.png, 운동기록.sql, and 운동기록.xlsx
</commit_message>
<xml_diff>
--- a/exercise/운동기록.xlsx
+++ b/exercise/운동기록.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Seung Jae Han\Dropbox\Trivia\운동기록\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8FC5E57-0341-47F6-AD96-3DEA0E9D67F2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFF0422A-C2DB-4B45-A536-24D2CCAA47FA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="18">
   <si>
     <t>DATETIME</t>
   </si>
@@ -441,11 +441,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L30"/>
+  <dimension ref="A1:L31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
+      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K31" sqref="K31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1598,6 +1598,44 @@
         <v>16</v>
       </c>
     </row>
+    <row r="31" spans="1:12">
+      <c r="A31" s="2">
+        <v>44016</v>
+      </c>
+      <c r="B31" s="3">
+        <v>98.7</v>
+      </c>
+      <c r="C31" s="3">
+        <v>105</v>
+      </c>
+      <c r="D31" s="3">
+        <v>0.94</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F31" s="3">
+        <v>0</v>
+      </c>
+      <c r="G31" s="3">
+        <v>81.900000000000006</v>
+      </c>
+      <c r="H31" s="3">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="I31" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J31" s="3">
+        <v>0</v>
+      </c>
+      <c r="K31" s="3">
+        <v>28.4</v>
+      </c>
+      <c r="L31" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>